<commit_message>
Simplification: remoived bidirectional_precise from Battery_Storage and El_network_onshore
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/network_data/line_cost_coefficients.xlsx
+++ b/dati_casoStudioItalia/network_data/line_cost_coefficients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ternaspa-my.sharepoint.com/personal/luca_santo_terna_it/Documents/Desktop/Altro/DRIN/Mix_Energetico/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\network_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151870" documentId="13_ncr:1_{DA97F3BF-9A5F-447D-A5F5-FAB025809DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B53ACA7B-54FF-4D11-A877-25CA2149573A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297951F7-27B4-4AF8-8AD6-A0EBB2AB481D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="riassunto" sheetId="3" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>y1</t>
   </si>
@@ -273,6 +273,18 @@
   </si>
   <si>
     <t>k€/(MW*km)</t>
+  </si>
+  <si>
+    <t>€</t>
+  </si>
+  <si>
+    <t>€/MW</t>
+  </si>
+  <si>
+    <t>€/km</t>
+  </si>
+  <si>
+    <t>€/(MW*km)</t>
   </si>
 </sst>
 </file>
@@ -342,14 +354,14 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -693,19 +705,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB09A16-0C24-4041-B50D-30183FB253D3}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>300000</v>
       </c>
@@ -733,7 +747,7 @@
         <v>3.3333327936166528</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -747,8 +761,55 @@
         <v>62</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>A2*10^3</f>
+        <v>300000000</v>
+      </c>
+      <c r="B8">
+        <f>B2*10^3</f>
+        <v>200000</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="B8:D8" si="0">C2*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3333.3327936166529</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -760,18 +821,18 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="19.28515625" customWidth="1"/>
-    <col min="14" max="14" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="88.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -815,7 +876,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -867,7 +928,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -916,7 +977,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -965,7 +1026,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1014,7 +1075,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1049,20 +1110,20 @@
         <v>1299999.8769445969</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>300000</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>200</v>
       </c>
-      <c r="G8" s="8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="8">
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
         <v>3.3333327936166528</v>
       </c>
       <c r="L8" t="s">
@@ -1073,7 +1134,7 @@
         <v>2.5640921849356249E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="L9" t="s">
         <v>49</v>
       </c>
@@ -1085,17 +1146,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="255" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="216" x14ac:dyDescent="0.3">
       <c r="N10" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>53</v>
       </c>
@@ -1109,17 +1170,17 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E13" s="5">
         <f>E2</f>
         <v>300000</v>
       </c>
       <c r="F13" s="5">
-        <f>F2*C2</f>
+        <f t="shared" ref="F13:G16" si="5">F2*C2</f>
         <v>200000</v>
       </c>
       <c r="G13" s="5">
-        <f>G2*D2</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H13" s="5">
@@ -1127,17 +1188,17 @@
         <v>3233332.8098081532</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E14" s="5">
         <f>E3</f>
         <v>300000</v>
       </c>
       <c r="F14" s="5">
-        <f>F3*C3</f>
+        <f t="shared" si="5"/>
         <v>100000</v>
       </c>
       <c r="G14" s="5">
-        <f>G3*D3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H14" s="5">
@@ -1145,17 +1206,17 @@
         <v>333333.27936166531</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E15" s="5">
         <f>E4</f>
         <v>300000</v>
       </c>
       <c r="F15" s="5">
-        <f>F4*C4</f>
+        <f t="shared" si="5"/>
         <v>200000</v>
       </c>
       <c r="G15" s="5">
-        <f>G4*D4</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H15" s="5">
@@ -1163,17 +1224,17 @@
         <v>833333.19840416324</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E16" s="5">
         <f>E5</f>
         <v>300000</v>
       </c>
       <c r="F16" s="5">
-        <f>F5*C5</f>
+        <f t="shared" si="5"/>
         <v>120000</v>
       </c>
       <c r="G16" s="5">
-        <f>G5*D5</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H16" s="5">
@@ -1181,7 +1242,7 @@
         <v>439999.92875739816</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>54</v>
       </c>
@@ -1190,81 +1251,81 @@
         <v>8.035715412562329E-2</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" ref="F17:H17" si="5">F13/(SUM($E13:$H13))</f>
+        <f t="shared" ref="F17:H17" si="6">F13/(SUM($E13:$H13))</f>
         <v>5.3571436083748855E-2</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.86607140979062791</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E18" s="6">
-        <f t="shared" ref="E18:H18" si="6">E14/(SUM($E14:$H14))</f>
+        <f t="shared" ref="E18:H18" si="7">E14/(SUM($E14:$H14))</f>
         <v>0.40909093919907324</v>
       </c>
       <c r="F18" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.13636364639969109</v>
       </c>
       <c r="G18" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.45454541440123575</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E19" s="6">
-        <f t="shared" ref="E19:H19" si="7">E15/(SUM($E15:$H15))</f>
+        <f t="shared" ref="E19:H19" si="8">E15/(SUM($E15:$H15))</f>
         <v>0.22500002276929978</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.15000001517953318</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.62499996205116715</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E20" s="6">
-        <f t="shared" ref="E20:H20" si="8">E16/(SUM($E16:$H16))</f>
+        <f t="shared" ref="E20:H20" si="9">E16/(SUM($E16:$H16))</f>
         <v>0.34883723820008428</v>
       </c>
       <c r="F20" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.13953489528003371</v>
       </c>
       <c r="G20" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.51162786651988201</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="7" t="s">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C22" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>0</v>
       </c>
@@ -1278,7 +1339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>409107.04084647918</v>
       </c>
@@ -1309,27 +1370,27 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="74.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="74.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1349,7 +1410,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1373,7 +1434,7 @@
         <v>4.2941666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1397,7 +1458,7 @@
         <v>91.454166666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1421,7 +1482,7 @@
         <v>3.6880000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>19</v>
       </c>
@@ -1429,7 +1490,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
         <v>20</v>
       </c>
@@ -1440,7 +1501,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1509,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>22</v>
       </c>
@@ -1456,7 +1517,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
         <v>23</v>
       </c>
@@ -1464,7 +1525,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>24</v>
       </c>
@@ -1472,7 +1533,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
         <v>31</v>
       </c>
@@ -1480,7 +1541,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
         <v>32</v>
       </c>
@@ -1488,7 +1549,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
         <v>33</v>
       </c>

</xml_diff>